<commit_message>
Add analyze swap part 1
</commit_message>
<xml_diff>
--- a/Analyze/planilha-numero-de-trocas.xlsx
+++ b/Analyze/planilha-numero-de-trocas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Trabalho\Mestrado - Ciência da Computação - Unesp\Disciplinas\Analise e Projeto de Algoritmos\Trabalhos\TP1\Sorting-Algorithms-Analysis-Complexity\Analyze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6820A1B8-6B6A-42DB-8DED-283B0901E9DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CF4BD51E-ABFE-4B68-86A8-D593FB2BF5C9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22200" windowHeight="9732" tabRatio="978" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
     <numFmt numFmtId="165" formatCode="0.00000000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -87,6 +87,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -204,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -241,13 +248,15 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11119,8 +11128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11169,13 +11178,21 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="B3" s="33">
+        <v>16</v>
+      </c>
+      <c r="C3" s="33">
+        <v>2371</v>
+      </c>
+      <c r="D3" s="33">
+        <v>249127</v>
+      </c>
+      <c r="E3" s="33">
+        <v>24901016</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
@@ -11190,13 +11207,21 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="8"/>
+      <c r="B4" s="33">
+        <v>16</v>
+      </c>
+      <c r="C4" s="33">
+        <v>2371</v>
+      </c>
+      <c r="D4" s="33">
+        <v>249127</v>
+      </c>
+      <c r="E4" s="33">
+        <v>24901016</v>
+      </c>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
@@ -11211,13 +11236,21 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="8"/>
+      <c r="B5" s="33">
+        <v>12</v>
+      </c>
+      <c r="C5" s="33">
+        <v>159</v>
+      </c>
+      <c r="D5" s="33">
+        <v>2408</v>
+      </c>
+      <c r="E5" s="33">
+        <v>31390</v>
+      </c>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="21"/>
       <c r="J5" s="22"/>
       <c r="K5" s="21"/>
@@ -11232,13 +11265,21 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="33">
+        <v>12</v>
+      </c>
+      <c r="C6" s="33">
+        <v>188</v>
+      </c>
+      <c r="D6" s="33">
+        <v>2674</v>
+      </c>
+      <c r="E6" s="33">
+        <v>34066</v>
+      </c>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="K6" s="21"/>
@@ -11253,13 +11294,21 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="B7" s="33">
+        <v>16</v>
+      </c>
+      <c r="C7" s="33">
+        <v>2371</v>
+      </c>
+      <c r="D7" s="33">
+        <v>249127</v>
+      </c>
+      <c r="E7" s="33">
+        <v>24901016</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="22"/>
@@ -11274,13 +11323,21 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="B8" s="33">
+        <v>9</v>
+      </c>
+      <c r="C8" s="33">
+        <v>314</v>
+      </c>
+      <c r="D8" s="33">
+        <v>7190</v>
+      </c>
+      <c r="E8" s="33">
+        <v>212680</v>
+      </c>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
@@ -11295,13 +11352,21 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="16"/>
+      <c r="B9" s="33">
+        <v>8</v>
+      </c>
+      <c r="C9" s="33">
+        <v>93</v>
+      </c>
+      <c r="D9" s="33">
+        <v>994</v>
+      </c>
+      <c r="E9" s="33">
+        <v>9981</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="35"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
@@ -11316,13 +11381,21 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="5"/>
+      <c r="B10" s="33">
+        <v>34</v>
+      </c>
+      <c r="C10" s="33">
+        <v>672</v>
+      </c>
+      <c r="D10" s="33">
+        <v>9976</v>
+      </c>
+      <c r="E10" s="33">
+        <v>133616</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
       <c r="I10" s="21"/>
       <c r="J10" s="22"/>
       <c r="K10" s="21"/>
@@ -11337,13 +11410,21 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="5"/>
+      <c r="B11" s="33">
+        <v>29</v>
+      </c>
+      <c r="C11" s="33">
+        <v>581</v>
+      </c>
+      <c r="D11" s="33">
+        <v>9096</v>
+      </c>
+      <c r="E11" s="33">
+        <v>124299</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="21"/>
       <c r="J11" s="22"/>
       <c r="K11" s="21"/>
@@ -11355,6 +11436,7 @@
       <c r="Q11" s="21"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="40"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
@@ -11422,7 +11504,9 @@
       <c r="F14" s="34">
         <v>0</v>
       </c>
-      <c r="G14" s="34"/>
+      <c r="G14" s="34">
+        <v>0</v>
+      </c>
       <c r="H14" s="33">
         <v>0</v>
       </c>
@@ -11455,7 +11539,9 @@
       <c r="F15" s="34">
         <v>0</v>
       </c>
-      <c r="G15" s="34"/>
+      <c r="G15" s="34">
+        <v>0</v>
+      </c>
       <c r="H15" s="33">
         <v>0</v>
       </c>
@@ -11474,32 +11560,32 @@
         <v>3</v>
       </c>
       <c r="B16" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C16" s="33">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D16" s="33">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E16" s="33">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="F16" s="34">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="G16" s="34">
-        <v>250000</v>
+        <v>500000</v>
       </c>
       <c r="H16" s="33">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="39">
         <v>6</v>
       </c>
       <c r="C17" s="33">
@@ -11514,9 +11600,11 @@
       <c r="F17" s="34">
         <v>65535</v>
       </c>
-      <c r="G17" s="34"/>
+      <c r="G17" s="34">
+        <v>262143</v>
+      </c>
       <c r="H17" s="33">
-        <v>262143</v>
+        <v>524287</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -11538,7 +11626,9 @@
       <c r="F18" s="33">
         <v>0</v>
       </c>
-      <c r="G18" s="33"/>
+      <c r="G18" s="33">
+        <v>0</v>
+      </c>
       <c r="H18" s="35">
         <v>0</v>
       </c>
@@ -11562,7 +11652,9 @@
       <c r="F19" s="33">
         <v>0</v>
       </c>
-      <c r="G19" s="33"/>
+      <c r="G19" s="33">
+        <v>0</v>
+      </c>
       <c r="H19" s="33">
         <v>0</v>
       </c>
@@ -11586,7 +11678,9 @@
       <c r="F20" s="33">
         <v>0</v>
       </c>
-      <c r="G20" s="33"/>
+      <c r="G20" s="33">
+        <v>0</v>
+      </c>
       <c r="H20" s="35">
         <v>0</v>
       </c>
@@ -11595,13 +11689,27 @@
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
+      <c r="B21" s="33">
+        <v>34</v>
+      </c>
+      <c r="C21" s="33">
+        <v>672</v>
+      </c>
+      <c r="D21" s="33">
+        <v>9976</v>
+      </c>
+      <c r="E21" s="33">
+        <v>133616</v>
+      </c>
+      <c r="F21" s="33">
+        <v>1668928</v>
+      </c>
+      <c r="G21" s="33">
+        <v>9475712</v>
+      </c>
+      <c r="H21" s="33">
+        <v>19951424</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -11622,9 +11730,11 @@
       <c r="F22" s="33">
         <v>1650886</v>
       </c>
-      <c r="G22" s="33"/>
+      <c r="G22" s="33">
+        <v>9355690</v>
+      </c>
       <c r="H22" s="33">
-        <v>9355690</v>
+        <v>19794250</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -11675,7 +11785,9 @@
       <c r="G25" s="33">
         <v>445698416</v>
       </c>
-      <c r="H25" s="33"/>
+      <c r="H25" s="33">
+        <v>1783293664</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -11696,7 +11808,9 @@
       <c r="F26" s="33">
         <v>704982704</v>
       </c>
-      <c r="G26" s="33"/>
+      <c r="G26" s="33">
+        <v>445698416</v>
+      </c>
       <c r="H26" s="33"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -11704,22 +11818,26 @@
         <v>3</v>
       </c>
       <c r="B27" s="33">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C27" s="33">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="D27" s="33">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="E27" s="33">
-        <v>0</v>
+        <v>9999</v>
       </c>
       <c r="F27" s="33">
-        <v>0</v>
-      </c>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
+        <v>99999</v>
+      </c>
+      <c r="G27" s="33">
+        <v>500000</v>
+      </c>
+      <c r="H27" s="33">
+        <v>999999</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -11728,7 +11846,7 @@
       <c r="B28" s="33">
         <v>11</v>
       </c>
-      <c r="C28" s="38">
+      <c r="C28" s="36">
         <v>112</v>
       </c>
       <c r="D28" s="33">
@@ -11740,14 +11858,18 @@
       <c r="F28" s="33">
         <v>115534</v>
       </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
+      <c r="G28" s="33">
+        <v>512142</v>
+      </c>
+      <c r="H28" s="33">
+        <v>1024286</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29" s="36">
         <v>45</v>
       </c>
       <c r="C29" s="33">
@@ -11762,8 +11884,12 @@
       <c r="F29" s="33">
         <v>704982704</v>
       </c>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
+      <c r="G29" s="33">
+        <v>445698416</v>
+      </c>
+      <c r="H29" s="33">
+        <v>1783293664</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -11784,8 +11910,12 @@
       <c r="F30" s="33">
         <v>19758228</v>
       </c>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
+      <c r="G30" s="33">
+        <v>499071604</v>
+      </c>
+      <c r="H30" s="33">
+        <v>1962492188</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
@@ -11806,20 +11936,38 @@
       <c r="F31" s="33">
         <v>50000</v>
       </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="35"/>
+      <c r="G31" s="33">
+        <v>250000</v>
+      </c>
+      <c r="H31" s="35">
+        <v>500000</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
+      <c r="B32" s="33">
+        <v>34</v>
+      </c>
+      <c r="C32" s="36">
+        <v>672</v>
+      </c>
+      <c r="D32" s="33">
+        <v>9976</v>
+      </c>
+      <c r="E32" s="33">
+        <v>133616</v>
+      </c>
+      <c r="F32" s="33">
+        <v>1668928</v>
+      </c>
+      <c r="G32" s="33">
+        <v>9475712</v>
+      </c>
+      <c r="H32" s="33">
+        <v>19951424</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
@@ -11838,21 +11986,25 @@
         <v>116722</v>
       </c>
       <c r="F33" s="33">
+        <v>1497466</v>
+      </c>
+      <c r="G33" s="33">
         <v>8668486</v>
       </c>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
+      <c r="H33" s="33">
+        <v>18333446</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -12679,6 +12831,102 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{B2CFF243-B058-42AF-B93F-E6B78D00A06A}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Geral!B60:I60</xm:f>
+              <xm:sqref>J60</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B61:I61</xm:f>
+              <xm:sqref>J61</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B62:I62</xm:f>
+              <xm:sqref>J62</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B63:I63</xm:f>
+              <xm:sqref>J63</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B64:I64</xm:f>
+              <xm:sqref>J64</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B65:I65</xm:f>
+              <xm:sqref>J65</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B66:I66</xm:f>
+              <xm:sqref>J66</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B67:I67</xm:f>
+              <xm:sqref>J67</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B68:I68</xm:f>
+              <xm:sqref>J68</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{E3264806-B52B-4012-8588-D9BE752B264E}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Geral!B49:I49</xm:f>
+              <xm:sqref>J49</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B50:I50</xm:f>
+              <xm:sqref>J50</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B51:I51</xm:f>
+              <xm:sqref>J51</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B52:I52</xm:f>
+              <xm:sqref>J52</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B53:I53</xm:f>
+              <xm:sqref>J53</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B54:I54</xm:f>
+              <xm:sqref>J54</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B55:I55</xm:f>
+              <xm:sqref>J55</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B56:I56</xm:f>
+              <xm:sqref>J56</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B57:I57</xm:f>
+              <xm:sqref>J57</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{667851D9-0D10-465D-B744-F05C0C2F3516}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -12731,102 +12979,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{E3264806-B52B-4012-8588-D9BE752B264E}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Geral!B49:I49</xm:f>
-              <xm:sqref>J49</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B50:I50</xm:f>
-              <xm:sqref>J50</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B51:I51</xm:f>
-              <xm:sqref>J51</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B52:I52</xm:f>
-              <xm:sqref>J52</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B53:I53</xm:f>
-              <xm:sqref>J53</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B54:I54</xm:f>
-              <xm:sqref>J54</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B55:I55</xm:f>
-              <xm:sqref>J55</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B56:I56</xm:f>
-              <xm:sqref>J56</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B57:I57</xm:f>
-              <xm:sqref>J57</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{B2CFF243-B058-42AF-B93F-E6B78D00A06A}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Geral!B60:I60</xm:f>
-              <xm:sqref>J60</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B61:I61</xm:f>
-              <xm:sqref>J61</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B62:I62</xm:f>
-              <xm:sqref>J62</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B63:I63</xm:f>
-              <xm:sqref>J63</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B64:I64</xm:f>
-              <xm:sqref>J64</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B65:I65</xm:f>
-              <xm:sqref>J65</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B66:I66</xm:f>
-              <xm:sqref>J66</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B67:I67</xm:f>
-              <xm:sqref>J67</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B68:I68</xm:f>
-              <xm:sqref>J68</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Add analyze swap part 3
</commit_message>
<xml_diff>
--- a/Analyze/planilha-numero-de-trocas.xlsx
+++ b/Analyze/planilha-numero-de-trocas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Trabalho\Mestrado - Ciência da Computação - Unesp\Disciplinas\Analise e Projeto de Algoritmos\Trabalhos\TP1\Sorting-Algorithms-Analysis-Complexity\Analyze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1E46B5DC-2FCC-4BF7-9139-800F1AB4A54C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9658BA25-0E61-487E-B319-37125A528285}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{FD045B66-2534-4FB9-AA69-2B06C69098A7}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,9 @@
       <c r="G4" s="2">
         <v>2375793494</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>766923805</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -637,7 +639,9 @@
       <c r="G5" s="2">
         <v>2375793494</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>766923805</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -661,7 +665,9 @@
       <c r="G6" s="2">
         <v>2187822</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>4396665</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -685,7 +691,9 @@
       <c r="G7" s="2">
         <v>2634364</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>5716509</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1157,7 +1165,9 @@
       <c r="G27" s="2">
         <v>445698416</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2">
+        <v>1783293664</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -1349,7 +1359,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{38FB41C9-CC1A-48DA-AC7E-73463EDE9753}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{CF4AD522-03A7-400B-B9D7-FA2E58BFCD5F}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1360,40 +1370,40 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Geral!B4:H4</xm:f>
-              <xm:sqref>I4</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B5:H5</xm:f>
-              <xm:sqref>I5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B6:H6</xm:f>
-              <xm:sqref>I6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B7:H7</xm:f>
-              <xm:sqref>I7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B8:H8</xm:f>
-              <xm:sqref>I8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B9:H9</xm:f>
-              <xm:sqref>I9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B10:H10</xm:f>
-              <xm:sqref>I10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B11:H11</xm:f>
-              <xm:sqref>I11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B12:H12</xm:f>
-              <xm:sqref>I12</xm:sqref>
+              <xm:f>Geral!B15:H15</xm:f>
+              <xm:sqref>I15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B16:H16</xm:f>
+              <xm:sqref>I16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B17:H17</xm:f>
+              <xm:sqref>I17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B18:H18</xm:f>
+              <xm:sqref>I18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B19:H19</xm:f>
+              <xm:sqref>I19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B20:H20</xm:f>
+              <xm:sqref>I20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B21:H21</xm:f>
+              <xm:sqref>I21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B22:H22</xm:f>
+              <xm:sqref>I22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B23:H23</xm:f>
+              <xm:sqref>I23</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1445,7 +1455,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{CF4AD522-03A7-400B-B9D7-FA2E58BFCD5F}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{38FB41C9-CC1A-48DA-AC7E-73463EDE9753}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1456,40 +1466,40 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Geral!B15:H15</xm:f>
-              <xm:sqref>I15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B16:H16</xm:f>
-              <xm:sqref>I16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B17:H17</xm:f>
-              <xm:sqref>I17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B18:H18</xm:f>
-              <xm:sqref>I18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B19:H19</xm:f>
-              <xm:sqref>I19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B20:H20</xm:f>
-              <xm:sqref>I20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B21:H21</xm:f>
-              <xm:sqref>I21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B22:H22</xm:f>
-              <xm:sqref>I22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Geral!B23:H23</xm:f>
-              <xm:sqref>I23</xm:sqref>
+              <xm:f>Geral!B4:H4</xm:f>
+              <xm:sqref>I4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B5:H5</xm:f>
+              <xm:sqref>I5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B6:H6</xm:f>
+              <xm:sqref>I6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B7:H7</xm:f>
+              <xm:sqref>I7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B8:H8</xm:f>
+              <xm:sqref>I8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B9:H9</xm:f>
+              <xm:sqref>I9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B10:H10</xm:f>
+              <xm:sqref>I10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B11:H11</xm:f>
+              <xm:sqref>I11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B12:H12</xm:f>
+              <xm:sqref>I12</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
Adding correct in article
</commit_message>
<xml_diff>
--- a/Analyze/planilha-numero-de-trocas.xlsx
+++ b/Analyze/planilha-numero-de-trocas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Trabalho\Mestrado - Ciência da Computação - Unesp\Disciplinas\Analise e Projeto de Algoritmos\Trabalhos\TP1\Sorting-Algorithms-Analysis-Complexity\Analyze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F5ED2603-006D-484E-A234-8B665ED650A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{16D98E7D-D332-4AA2-974A-D3164A6E2904}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{FD045B66-2534-4FB9-AA69-2B06C69098A7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{FD045B66-2534-4FB9-AA69-2B06C69098A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -188,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -221,6 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D0673C-47FA-4992-B60E-B81B80C6E1BD}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1188,7 @@
       <c r="C28" s="2">
         <v>99</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="18">
         <v>999</v>
       </c>
       <c r="E28" s="2">
@@ -1356,10 +1365,11 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{38FB41C9-CC1A-48DA-AC7E-73463EDE9753}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{CF4AD522-03A7-400B-B9D7-FA2E58BFCD5F}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1370,40 +1380,40 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Geral!B4:H4</xm:f>
-              <xm:sqref>I4</xm:sqref>
+              <xm:f>Geral!B15:H15</xm:f>
+              <xm:sqref>I15</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B5:H5</xm:f>
-              <xm:sqref>I5</xm:sqref>
+              <xm:f>Geral!B16:H16</xm:f>
+              <xm:sqref>I16</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B6:H6</xm:f>
-              <xm:sqref>I6</xm:sqref>
+              <xm:f>Geral!B17:H17</xm:f>
+              <xm:sqref>I17</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B7:H7</xm:f>
-              <xm:sqref>I7</xm:sqref>
+              <xm:f>Geral!B18:H18</xm:f>
+              <xm:sqref>I18</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B8:H8</xm:f>
-              <xm:sqref>I8</xm:sqref>
+              <xm:f>Geral!B19:H19</xm:f>
+              <xm:sqref>I19</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B9:H9</xm:f>
-              <xm:sqref>I9</xm:sqref>
+              <xm:f>Geral!B20:H20</xm:f>
+              <xm:sqref>I20</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B10:H10</xm:f>
-              <xm:sqref>I10</xm:sqref>
+              <xm:f>Geral!B21:H21</xm:f>
+              <xm:sqref>I21</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B11:H11</xm:f>
-              <xm:sqref>I11</xm:sqref>
+              <xm:f>Geral!B22:H22</xm:f>
+              <xm:sqref>I22</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B12:H12</xm:f>
-              <xm:sqref>I12</xm:sqref>
+              <xm:f>Geral!B23:H23</xm:f>
+              <xm:sqref>I23</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1455,7 +1465,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{CF4AD522-03A7-400B-B9D7-FA2E58BFCD5F}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{38FB41C9-CC1A-48DA-AC7E-73463EDE9753}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1466,40 +1476,40 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Geral!B15:H15</xm:f>
-              <xm:sqref>I15</xm:sqref>
+              <xm:f>Geral!B4:H4</xm:f>
+              <xm:sqref>I4</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B16:H16</xm:f>
-              <xm:sqref>I16</xm:sqref>
+              <xm:f>Geral!B5:H5</xm:f>
+              <xm:sqref>I5</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B17:H17</xm:f>
-              <xm:sqref>I17</xm:sqref>
+              <xm:f>Geral!B6:H6</xm:f>
+              <xm:sqref>I6</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B18:H18</xm:f>
-              <xm:sqref>I18</xm:sqref>
+              <xm:f>Geral!B7:H7</xm:f>
+              <xm:sqref>I7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B19:H19</xm:f>
-              <xm:sqref>I19</xm:sqref>
+              <xm:f>Geral!B8:H8</xm:f>
+              <xm:sqref>I8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B20:H20</xm:f>
-              <xm:sqref>I20</xm:sqref>
+              <xm:f>Geral!B9:H9</xm:f>
+              <xm:sqref>I9</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B21:H21</xm:f>
-              <xm:sqref>I21</xm:sqref>
+              <xm:f>Geral!B10:H10</xm:f>
+              <xm:sqref>I10</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B22:H22</xm:f>
-              <xm:sqref>I22</xm:sqref>
+              <xm:f>Geral!B11:H11</xm:f>
+              <xm:sqref>I11</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Geral!B23:H23</xm:f>
-              <xm:sqref>I23</xm:sqref>
+              <xm:f>Geral!B12:H12</xm:f>
+              <xm:sqref>I12</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -1645,7 +1655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C002D5DC-E0BD-4358-A613-55A50C96D005}">
   <dimension ref="A3:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correction in the number swap file
</commit_message>
<xml_diff>
--- a/Analyze/planilha-numero-de-trocas.xlsx
+++ b/Analyze/planilha-numero-de-trocas.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\traballho01-Bruno-Leandro\Planilhas Experimento\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F8EBCD01-96FA-4368-85CB-78AC604A58D1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="10766" windowHeight="9259"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10764" windowHeight="9264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
   <si>
     <t>Análise número de trocas</t>
   </si>
@@ -70,14 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,152 +105,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,19 +115,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399945066682943"/>
+        <fgColor theme="8" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399945066682943"/>
+        <fgColor theme="5" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,192 +139,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799951170384838"/>
+        <fgColor theme="8" tint="0.79992065187536243"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -504,251 +186,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -768,9 +208,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,63 +217,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -845,7 +246,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="5C616C"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1097,61 +498,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.3283582089552" customWidth="1"/>
-    <col min="2" max="2" width="13.4402985074627" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="13.5522388059701" customWidth="1"/>
-    <col min="5" max="5" width="13.4402985074627" customWidth="1"/>
-    <col min="6" max="7" width="13.3283582089552" customWidth="1"/>
-    <col min="8" max="8" width="13.7761194029851" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>10</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>100</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>1000</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>10000</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>100000</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>500000</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>1000000</v>
       </c>
     </row>
@@ -1177,7 +577,7 @@
       <c r="G4" s="7">
         <v>62476565906</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <v>249875026973</v>
       </c>
     </row>
@@ -1203,7 +603,7 @@
       <c r="G5" s="7">
         <v>62476565906</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>249875026973</v>
       </c>
     </row>
@@ -1333,7 +733,7 @@
       <c r="G10" s="7">
         <v>499968</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <v>999957</v>
       </c>
     </row>
@@ -1389,35 +789,35 @@
         <v>19048402</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="11"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+    <row r="13" spans="1:8">
+      <c r="B13" s="10"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>10</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>100</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>1000</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>10000</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>100000</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>500000</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>1000000</v>
       </c>
     </row>
@@ -1437,10 +837,10 @@
       <c r="E15" s="7">
         <v>0</v>
       </c>
-      <c r="F15" s="18">
-        <v>0</v>
-      </c>
-      <c r="G15" s="18">
+      <c r="F15" s="17">
+        <v>0</v>
+      </c>
+      <c r="G15" s="17">
         <v>0</v>
       </c>
       <c r="H15" s="7">
@@ -1463,10 +863,10 @@
       <c r="E16" s="7">
         <v>0</v>
       </c>
-      <c r="F16" s="18">
-        <v>0</v>
-      </c>
-      <c r="G16" s="18">
+      <c r="F16" s="17">
+        <v>0</v>
+      </c>
+      <c r="G16" s="17">
         <v>0</v>
       </c>
       <c r="H16" s="7">
@@ -1489,10 +889,10 @@
       <c r="E17" s="7">
         <v>10000</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="17">
         <v>100000</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="17">
         <v>500000</v>
       </c>
       <c r="H17" s="7">
@@ -1503,7 +903,7 @@
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>6</v>
       </c>
       <c r="C18" s="7">
@@ -1515,10 +915,10 @@
       <c r="E18" s="7">
         <v>5904</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="17">
         <v>65535</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="17">
         <v>262143</v>
       </c>
       <c r="H18" s="7">
@@ -1547,7 +947,7 @@
       <c r="G19" s="7">
         <v>0</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="15">
         <v>0</v>
       </c>
     </row>
@@ -1599,7 +999,7 @@
       <c r="G21" s="7">
         <v>0</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="15">
         <v>0</v>
       </c>
     </row>
@@ -1656,28 +1056,28 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>10</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="9">
         <v>100</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>1000</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="9">
         <v>10000</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="9">
         <v>100000</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="9">
         <v>500000</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="9">
         <v>1000000</v>
       </c>
     </row>
@@ -1766,7 +1166,7 @@
       <c r="B29" s="7">
         <v>11</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="12">
         <v>112</v>
       </c>
       <c r="D29" s="7">
@@ -1789,7 +1189,7 @@
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="12">
         <v>45</v>
       </c>
       <c r="C30" s="7">
@@ -1859,7 +1259,7 @@
       <c r="G32" s="7">
         <v>250000</v>
       </c>
-      <c r="H32" s="16">
+      <c r="H32" s="15">
         <v>500000</v>
       </c>
     </row>
@@ -1870,7 +1270,7 @@
       <c r="B33" s="7">
         <v>34</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="12">
         <v>672</v>
       </c>
       <c r="D33" s="7">
@@ -1919,25 +1319,174 @@
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D13E861C-DD6E-4B2F-B4AD-0BB18A56890C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Geral!B26:H26</xm:f>
+              <xm:sqref>I26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B27:H27</xm:f>
+              <xm:sqref>I27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B28:H28</xm:f>
+              <xm:sqref>I28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B29:H29</xm:f>
+              <xm:sqref>I29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B30:H30</xm:f>
+              <xm:sqref>I30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B31:H31</xm:f>
+              <xm:sqref>I31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B32:H32</xm:f>
+              <xm:sqref>I32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B33:H33</xm:f>
+              <xm:sqref>I33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B34:H34</xm:f>
+              <xm:sqref>I34</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{04DD6297-083E-4B62-AC19-C90FDD76B865}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Geral!B15:H15</xm:f>
+              <xm:sqref>I15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B16:H16</xm:f>
+              <xm:sqref>I16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B17:H17</xm:f>
+              <xm:sqref>I17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B18:H18</xm:f>
+              <xm:sqref>I18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B19:H19</xm:f>
+              <xm:sqref>I19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B20:H20</xm:f>
+              <xm:sqref>I20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B21:H21</xm:f>
+              <xm:sqref>I21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B22:H22</xm:f>
+              <xm:sqref>I22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B23:H23</xm:f>
+              <xm:sqref>I23</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{B06E0B5E-EAB3-4AC8-A327-44A8F1773A9E}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Geral!B4:H4</xm:f>
+              <xm:sqref>I4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B5:H5</xm:f>
+              <xm:sqref>I5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B6:H6</xm:f>
+              <xm:sqref>I6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B7:H7</xm:f>
+              <xm:sqref>I7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B8:H8</xm:f>
+              <xm:sqref>I8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B9:H9</xm:f>
+              <xm:sqref>I9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B10:H10</xm:f>
+              <xm:sqref>I10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B11:H11</xm:f>
+              <xm:sqref>I11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Geral!B12:H12</xm:f>
+              <xm:sqref>I12</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.4402985074627" customWidth="1"/>
-    <col min="2" max="2" width="13.2164179104478" customWidth="1"/>
-    <col min="3" max="4" width="13.4402985074627" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="4" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -2053,25 +1602,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.4402985074627" customWidth="1"/>
-    <col min="2" max="3" width="13.6641791044776" customWidth="1"/>
-    <col min="4" max="4" width="13.7761194029851" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -2155,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="7">
-        <v>704982704</v>
+        <v>4999950000</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2163,48 +1711,48 @@
         <v>500000</v>
       </c>
       <c r="B9" s="6">
-        <v>2375793494</v>
+        <v>62476565906</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
       </c>
       <c r="D9" s="7">
-        <v>445698416</v>
+        <v>124999750000</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5">
         <v>1000000</v>
       </c>
-      <c r="B10" s="6">
-        <v>766923805</v>
+      <c r="B10" s="14">
+        <v>249875026973</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10" s="7">
-        <v>1783293664</v>
+        <v>499999500000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.3283582089552" customWidth="1"/>
-    <col min="2" max="4" width="13.5522388059701" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -2288,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="7">
-        <v>704982704</v>
+        <v>4999950000</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2296,49 +1844,47 @@
         <v>500000</v>
       </c>
       <c r="B9" s="6">
-        <v>2375793494</v>
+        <v>62476565906</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
       </c>
       <c r="D9" s="7">
-        <v>445698416</v>
+        <v>124999750000</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5">
         <v>1000000</v>
       </c>
-      <c r="B10" s="6">
-        <v>766923805</v>
+      <c r="B10" s="14">
+        <v>249875026973</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10" s="7">
-        <v>1783293664</v>
+        <v>499999500000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.5522388059701" customWidth="1"/>
-    <col min="2" max="3" width="13.4402985074627" customWidth="1"/>
-    <col min="4" max="4" width="13.6641791044776" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -2454,26 +2000,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.6641791044776" customWidth="1"/>
-    <col min="3" max="3" width="13.4402985074627" customWidth="1"/>
-    <col min="4" max="4" width="13.2164179104478" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -2589,161 +2133,157 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A3:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A5:D12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.7761194029851" customWidth="1"/>
-    <col min="2" max="2" width="13.4402985074627" customWidth="1"/>
-    <col min="3" max="3" width="13.2164179104478" customWidth="1"/>
-    <col min="4" max="4" width="13.3283582089552" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5">
-        <v>100</v>
-      </c>
-      <c r="B5" s="6">
-        <v>2371</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
-        <v>4950</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="B6" s="6">
-        <v>249127</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6" s="7">
-        <v>499500</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="B7" s="6">
-        <v>24901016</v>
+        <v>2371</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7" s="7">
-        <v>49995000</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5">
-        <v>100000</v>
-      </c>
-      <c r="B8" s="8">
-        <v>2500023166</v>
+        <v>1000</v>
+      </c>
+      <c r="B8" s="6">
+        <v>249127</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
       </c>
       <c r="D8" s="7">
-        <v>704982704</v>
+        <v>499500</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5">
-        <v>500000</v>
+        <v>10000</v>
       </c>
       <c r="B9" s="6">
-        <v>2375793494</v>
+        <v>24901016</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
       </c>
       <c r="D9" s="7">
-        <v>445698416</v>
+        <v>49995000</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5">
+        <v>100000</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2500023166</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4999950000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="5">
+        <v>500000</v>
+      </c>
+      <c r="B11" s="6">
+        <v>62476565906</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>124999750000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="5">
         <v>1000000</v>
       </c>
-      <c r="B10" s="6">
-        <v>766923805</v>
-      </c>
-      <c r="C10" s="7">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7">
-        <v>1783293664</v>
+      <c r="B12" s="14">
+        <v>249875026973</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>499999500000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5522388059701" customWidth="1"/>
-    <col min="2" max="2" width="13.4402985074627" customWidth="1"/>
-    <col min="3" max="3" width="13.6641791044776" customWidth="1"/>
-    <col min="4" max="4" width="13.3283582089552" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -2859,26 +2399,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.3283582089552" customWidth="1"/>
-    <col min="2" max="2" width="13.6641791044776" customWidth="1"/>
-    <col min="3" max="3" width="13.4402985074627" customWidth="1"/>
-    <col min="4" max="4" width="13.3283582089552" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -2994,25 +2532,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.8880597014925" customWidth="1"/>
-    <col min="2" max="2" width="13.2164179104478" customWidth="1"/>
-    <col min="3" max="4" width="13.3283582089552" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -3128,7 +2664,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
-  <headerFooter/>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78680555555555598" bottom="0.78680555555555598" header="0.31388888888888899" footer="0.31388888888888899"/>
 </worksheet>
 </file>
</xml_diff>